<commit_message>
EPBDS-2602 Add toString(), toInteger(), toDouble(), toNumber(), toDate()
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Date.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Date.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.test\test\rules\functionality\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="14970" tabRatio="833" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="7" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="diff" sheetId="10" r:id="rId5"/>
     <sheet name="dateOfQuarter" sheetId="14" r:id="rId6"/>
     <sheet name="lastDayOfMonth" sheetId="25" r:id="rId7"/>
-    <sheet name="dateToString" sheetId="8" r:id="rId8"/>
+    <sheet name="toString" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -31,7 +26,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="L83" authorId="0" shapeId="0">
+    <comment ref="L83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +62,7 @@
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="I22" authorId="0" shapeId="0">
+    <comment ref="I22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I23" authorId="0" shapeId="0">
+    <comment ref="I23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +125,7 @@
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="C29" authorId="0" shapeId="0">
+    <comment ref="C29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +168,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +231,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="D68" authorId="0" shapeId="0">
+    <comment ref="D69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="186">
   <si>
     <t>_res_</t>
   </si>
@@ -315,9 +310,6 @@
     <t>Test dateToStringFormatMethod dateToStringFormatTest</t>
   </si>
   <si>
-    <t>return dateToString(date, dateFormat);</t>
-  </si>
-  <si>
     <t>dateFormat</t>
   </si>
   <si>
@@ -402,9 +394,6 @@
     <t>01/20/2001</t>
   </si>
   <si>
-    <t>1/20/01</t>
-  </si>
-  <si>
     <t>12/31/2014</t>
   </si>
   <si>
@@ -826,12 +815,18 @@
   </si>
   <si>
     <t>Method int dayDiffMethod (Date date1, Date date2)</t>
+  </si>
+  <si>
+    <t>return toString(date, dateFormat);</t>
+  </si>
+  <si>
+    <t>01/01/2001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
@@ -1080,7 +1075,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1475,19 +1470,19 @@
       </c>
       <c r="C2" s="35"/>
       <c r="E2" s="35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I2" s="35"/>
       <c r="K2" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L2" s="35"/>
       <c r="N2" s="35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O2" s="35"/>
     </row>
@@ -1497,19 +1492,19 @@
       </c>
       <c r="C3" s="36"/>
       <c r="E3" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F3" s="36"/>
       <c r="H3" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I3" s="36"/>
       <c r="K3" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L3" s="36"/>
       <c r="N3" s="36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O3" s="36"/>
     </row>
@@ -1519,19 +1514,19 @@
       </c>
       <c r="C5" s="38"/>
       <c r="E5" s="37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="38"/>
       <c r="H5" s="37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I5" s="38"/>
       <c r="K5" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L5" s="38"/>
       <c r="N5" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O5" s="38"/>
     </row>
@@ -1575,25 +1570,25 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>1</v>
@@ -1619,13 +1614,13 @@
         <v>0</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L8" s="10">
         <v>0</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O8" s="10">
         <v>0</v>
@@ -1651,13 +1646,13 @@
         <v>0</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O9" s="10">
         <v>0</v>
@@ -1683,13 +1678,13 @@
         <v>0</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L10" s="10">
         <v>0</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O10" s="10">
         <v>0</v>
@@ -1715,13 +1710,13 @@
         <v>1</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O11" s="10">
         <v>0</v>
@@ -1747,13 +1742,13 @@
         <v>1</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O12" s="10">
         <v>0</v>
@@ -1779,13 +1774,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O13" s="10">
         <v>0</v>
@@ -2756,7 +2751,7 @@
         <v>42197.499999999971</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E44" s="26">
         <v>42197.499999999971</v>
@@ -2788,7 +2783,7 @@
         <v>42197.500011574048</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E45" s="26">
         <v>42197.500011574048</v>
@@ -2820,7 +2815,7 @@
         <v>42197.541655092566</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E46" s="26">
         <v>42197.541655092566</v>
@@ -2852,7 +2847,7 @@
         <v>42197.541666666635</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E47" s="26">
         <v>42197.541666666635</v>
@@ -2884,7 +2879,7 @@
         <v>42197.541678240712</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E48" s="26">
         <v>42197.541678240712</v>
@@ -2916,7 +2911,7 @@
         <v>42197.58332175923</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E49" s="26">
         <v>42197.58332175923</v>
@@ -2948,7 +2943,7 @@
         <v>42197.583333333299</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E50" s="26">
         <v>42197.583333333299</v>
@@ -2980,7 +2975,7 @@
         <v>42197.583344907376</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E51" s="26">
         <v>42197.583344907376</v>
@@ -3012,7 +3007,7 @@
         <v>42197.624988425894</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E52" s="26">
         <v>42197.624988425894</v>
@@ -3044,7 +3039,7 @@
         <v>42197.624999999964</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E53" s="26">
         <v>42197.624999999964</v>
@@ -3076,7 +3071,7 @@
         <v>42197.62501157404</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E54" s="26">
         <v>42197.62501157404</v>
@@ -3108,7 +3103,7 @@
         <v>42197.666655092558</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E55" s="26">
         <v>42197.666655092558</v>
@@ -3140,7 +3135,7 @@
         <v>42197.666666666628</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E56" s="26">
         <v>42197.666666666628</v>
@@ -3172,7 +3167,7 @@
         <v>42197.666678240705</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E57" s="26">
         <v>42197.666678240705</v>
@@ -3204,7 +3199,7 @@
         <v>42197.708321759223</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E58" s="26">
         <v>42197.708321759223</v>
@@ -3236,7 +3231,7 @@
         <v>42197.708333333292</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E59" s="26">
         <v>42197.708333333292</v>
@@ -3268,7 +3263,7 @@
         <v>42197.708344907369</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E60" s="26">
         <v>42197.708344907369</v>
@@ -3300,7 +3295,7 @@
         <v>42197.749988425887</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E61" s="26">
         <v>42197.749988425887</v>
@@ -3332,7 +3327,7 @@
         <v>42197.749999999956</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E62" s="26">
         <v>42197.749999999956</v>
@@ -3364,7 +3359,7 @@
         <v>42197.750011574033</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E63" s="26">
         <v>42197.750011574033</v>
@@ -3396,7 +3391,7 @@
         <v>42197.791655092551</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E64" s="26">
         <v>42197.791655092551</v>
@@ -3428,7 +3423,7 @@
         <v>42197.791666666621</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E65" s="26">
         <v>42197.791666666621</v>
@@ -3460,7 +3455,7 @@
         <v>42197.791678240697</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E66" s="26">
         <v>42197.791678240697</v>
@@ -3492,7 +3487,7 @@
         <v>42197.833321759215</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E67" s="26">
         <v>42197.833321759215</v>
@@ -3524,7 +3519,7 @@
         <v>42197.833333333285</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E68" s="26">
         <v>42197.833333333285</v>
@@ -3556,7 +3551,7 @@
         <v>42197.833344907362</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E69" s="26">
         <v>42197.833344907362</v>
@@ -3588,7 +3583,7 @@
         <v>42197.87498842588</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E70" s="26">
         <v>42197.87498842588</v>
@@ -3620,7 +3615,7 @@
         <v>42197.874999999949</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E71" s="26">
         <v>42197.874999999949</v>
@@ -3652,7 +3647,7 @@
         <v>42197.875011574026</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E72" s="26">
         <v>42197.875011574026</v>
@@ -3684,7 +3679,7 @@
         <v>42197.916655092544</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E73" s="26">
         <v>42197.916655092544</v>
@@ -3716,7 +3711,7 @@
         <v>42197.916666666613</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E74" s="26">
         <v>42197.916666666613</v>
@@ -3748,7 +3743,7 @@
         <v>42197.91667824069</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E75" s="26">
         <v>42197.91667824069</v>
@@ -3780,7 +3775,7 @@
         <v>42197.958321759208</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E76" s="26">
         <v>42197.958321759208</v>
@@ -3812,7 +3807,7 @@
         <v>42197.958333333278</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E77" s="26">
         <v>42197.958333333278</v>
@@ -3844,7 +3839,7 @@
         <v>42197.958344907354</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E78" s="26">
         <v>42197.958344907354</v>
@@ -3876,7 +3871,7 @@
         <v>42197.999988425872</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E79" s="26">
         <v>42197.999988425872</v>
@@ -3905,7 +3900,7 @@
     </row>
     <row r="83" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K83" s="31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L83" s="30">
         <v>42</v>
@@ -3913,7 +3908,7 @@
     </row>
     <row r="84" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K84" s="31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L84" s="30">
         <v>30</v>
@@ -3921,7 +3916,7 @@
     </row>
     <row r="85" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K85" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L85" s="6">
         <v>0</v>
@@ -3971,43 +3966,43 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="35"/>
       <c r="E2" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="36"/>
       <c r="E3" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F3" s="36"/>
       <c r="H3" s="36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I3" s="36"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="38"/>
       <c r="E5" s="37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F5" s="38"/>
       <c r="H5" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I5" s="38"/>
     </row>
@@ -4033,13 +4028,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
@@ -4054,19 +4049,19 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10">
         <v>4</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8" s="10">
         <v>14</v>
@@ -4075,19 +4070,19 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I9" s="10">
         <v>30</v>
@@ -4096,19 +4091,19 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="11">
         <v>1789</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="10">
         <v>4</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I10" s="10">
         <v>14</v>
@@ -4117,19 +4112,19 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" s="10">
         <v>0</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" s="10">
         <v>1</v>
@@ -4137,19 +4132,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F12" s="10">
         <v>11</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I12" s="10">
         <v>30</v>
@@ -4157,19 +4152,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="11">
         <v>10</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I13" s="6">
         <v>1</v>
@@ -4197,19 +4192,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="11">
         <v>1899</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="10">
         <v>11</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="6">
         <v>31</v>
@@ -4217,19 +4212,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" s="11">
         <v>1899</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F16" s="10">
         <v>11</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I16" s="6">
         <v>30</v>
@@ -4237,19 +4232,19 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C17" s="11">
         <v>1894</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F17" s="10">
         <v>4</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I17" s="6">
         <v>25</v>
@@ -4277,19 +4272,19 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="13">
         <v>3892</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F19" s="10">
         <v>4</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I19" s="6">
         <v>14</v>
@@ -4339,67 +4334,67 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="35"/>
       <c r="E2" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I2" s="35"/>
       <c r="K2" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L2" s="35"/>
       <c r="N2" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="36"/>
       <c r="E3" s="36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" s="36"/>
       <c r="H3" s="36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I3" s="36"/>
       <c r="K3" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L3" s="36"/>
       <c r="N3" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O3" s="36"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="38"/>
       <c r="E5" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" s="38"/>
       <c r="H5" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I5" s="38"/>
       <c r="K5" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L5" s="38"/>
       <c r="N5" s="37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O5" s="38"/>
     </row>
@@ -4443,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
@@ -4455,13 +4450,13 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>1</v>
@@ -4470,31 +4465,31 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="10">
         <v>134</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="10">
         <v>5</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L8" s="10">
         <v>20</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O8" s="10">
         <v>3</v>
@@ -4503,13 +4498,13 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10">
         <v>364</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="10">
         <v>3</v>
@@ -4521,13 +4516,13 @@
         <v>5</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L9" s="10">
         <v>1</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O9" s="10">
         <v>5</v>
@@ -4536,31 +4531,31 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="10">
         <v>134</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="10">
         <v>1</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L10" s="10">
         <v>20</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O10" s="10">
         <v>3</v>
@@ -4569,31 +4564,31 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="10">
         <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" s="17">
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I11" s="10">
         <v>7</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L11" s="10">
         <v>1</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O11" s="10">
         <v>1</v>
@@ -4602,31 +4597,31 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="10">
         <v>364</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I12" s="10">
         <v>4</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L12" s="10">
         <v>1</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O12" s="10">
         <v>5</v>
@@ -4635,31 +4630,31 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="10">
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="17">
         <v>0</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I13" s="10">
         <v>5</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L13" s="10">
         <v>1</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O13" s="10">
         <v>1</v>
@@ -4680,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I14" s="20">
         <v>5</v>
@@ -4701,31 +4696,31 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="6">
         <v>365</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="10">
         <v>3</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I15" s="20">
         <v>4</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L15" s="10">
         <v>1</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O15" s="10">
         <v>6</v>
@@ -4734,13 +4729,13 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" s="16">
         <v>364</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F16" s="10">
         <v>3</v>
@@ -4752,13 +4747,13 @@
         <v>2</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L16" s="10">
         <v>52</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O16" s="10">
         <v>5</v>
@@ -4767,31 +4762,31 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C17" s="16">
         <v>145</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17" s="20">
         <v>1</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L17" s="10">
         <v>21</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O17" s="10">
         <v>4</v>
@@ -4812,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I18" s="20">
         <v>7</v>
@@ -4833,31 +4828,31 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="16">
         <v>135</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I19" s="20">
         <v>6</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L19" s="10">
         <v>20</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O19" s="10">
         <v>2</v>
@@ -4873,7 +4868,7 @@
       <c r="B21" s="32"/>
       <c r="C21" s="33"/>
       <c r="H21" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I21" s="10">
         <v>2</v>
@@ -4882,7 +4877,7 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="H22" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I22" s="20">
         <v>6</v>
@@ -4891,7 +4886,7 @@
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="H23" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I23" s="20">
         <v>2</v>
@@ -4950,7 +4945,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="35"/>
     </row>
@@ -5016,7 +5011,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="9">
         <v>120</v>
@@ -5048,7 +5043,7 @@
     </row>
     <row r="16" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" s="6">
         <v>46708</v>
@@ -5056,7 +5051,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C20" s="35"/>
     </row>
@@ -5090,7 +5085,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" s="16">
         <v>8061</v>
@@ -5098,7 +5093,7 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27" s="7">
         <v>8063</v>
@@ -5106,7 +5101,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="10">
         <v>7157</v>
@@ -5114,7 +5109,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29" s="6">
         <v>4</v>
@@ -5122,7 +5117,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="6">
         <v>8063</v>
@@ -5130,7 +5125,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" s="6">
         <v>40</v>
@@ -5146,7 +5141,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="6">
         <v>7599</v>
@@ -5154,7 +5149,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C34" s="6">
         <v>7599</v>
@@ -5162,7 +5157,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C35" s="6">
         <v>7577</v>
@@ -5178,7 +5173,7 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C37" s="6">
         <v>15569</v>
@@ -5204,7 +5199,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -5217,31 +5212,31 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="38"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
@@ -5249,10 +5244,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>1</v>
@@ -5260,10 +5255,10 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -5298,10 +5293,10 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
@@ -5309,10 +5304,10 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" s="10">
         <v>365</v>
@@ -5331,10 +5326,10 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" s="10">
         <v>364</v>
@@ -5342,10 +5337,10 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="21">
         <v>78891</v>
@@ -5361,7 +5356,7 @@
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="20">
         <v>0</v>
@@ -5369,7 +5364,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20">
@@ -5378,10 +5373,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D20" s="10">
         <v>-32872</v>
@@ -5389,10 +5384,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21" s="10">
         <v>32872</v>
@@ -5400,7 +5395,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" s="24">
         <v>1</v>
@@ -5411,7 +5406,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C23" s="23">
         <v>1</v>
@@ -5422,7 +5417,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" s="23">
         <v>2</v>
@@ -5444,31 +5439,31 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" s="39"/>
       <c r="D32" s="38"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>0</v>
@@ -5476,10 +5471,10 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>1</v>
@@ -5487,10 +5482,10 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D35" s="10">
         <v>0</v>
@@ -5498,10 +5493,10 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D36" s="10">
         <v>52</v>
@@ -5520,10 +5515,10 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D38" s="10">
         <v>52</v>
@@ -5531,10 +5526,10 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D39" s="21">
         <v>11270</v>
@@ -5550,7 +5545,7 @@
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="20">
         <v>0</v>
@@ -5558,7 +5553,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="20">
@@ -5567,10 +5562,10 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D43" s="10">
         <v>-4696</v>
@@ -5578,10 +5573,10 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D44" s="10">
         <v>4696</v>
@@ -5589,7 +5584,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="24">
         <v>1</v>
@@ -5600,7 +5595,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C46" s="23">
         <v>1</v>
@@ -5611,7 +5606,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C47" s="23">
         <v>2</v>
@@ -5633,31 +5628,31 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="35"/>
       <c r="D52" s="35"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C53" s="36"/>
       <c r="D53" s="36"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" s="39"/>
       <c r="D55" s="38"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>0</v>
@@ -5665,10 +5660,10 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>1</v>
@@ -5676,10 +5671,10 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D58" s="10">
         <v>0</v>
@@ -5687,10 +5682,10 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D59" s="10">
         <v>12</v>
@@ -5709,10 +5704,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D61" s="10">
         <v>12</v>
@@ -5720,10 +5715,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D62" s="21">
         <v>2591</v>
@@ -5739,7 +5734,7 @@
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="18"/>
       <c r="C64" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D64" s="20">
         <v>0</v>
@@ -5747,7 +5742,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="20">
@@ -5756,10 +5751,10 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D66" s="20">
         <v>-1080</v>
@@ -5767,10 +5762,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D67" s="20">
         <v>1080</v>
@@ -5778,7 +5773,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C68" s="24">
         <v>1</v>
@@ -5789,7 +5784,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C69" s="23">
         <v>1</v>
@@ -5800,7 +5795,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C70" s="23">
         <v>2</v>
@@ -5822,31 +5817,31 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C75" s="35"/>
       <c r="D75" s="35"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C76" s="36"/>
       <c r="D76" s="36"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C78" s="39"/>
       <c r="D78" s="38"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>0</v>
@@ -5854,10 +5849,10 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>1</v>
@@ -5865,10 +5860,10 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D81" s="10">
         <v>0</v>
@@ -5876,10 +5871,10 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D82" s="10">
         <v>1</v>
@@ -5898,10 +5893,10 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D84" s="10">
         <v>0</v>
@@ -5909,10 +5904,10 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D85" s="10">
         <v>215</v>
@@ -5928,7 +5923,7 @@
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="18"/>
       <c r="C87" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D87" s="20">
         <v>0</v>
@@ -5936,7 +5931,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C88" s="19"/>
       <c r="D88" s="20">
@@ -5945,10 +5940,10 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D89" s="10">
         <v>-90</v>
@@ -5956,10 +5951,10 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D90" s="10">
         <v>90</v>
@@ -6013,25 +6008,25 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="35"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="36"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="38"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -6039,7 +6034,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
@@ -6051,7 +6046,7 @@
         <v>8060</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -6060,7 +6055,7 @@
         <v>8061</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -6069,7 +6064,7 @@
         <v>8062</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6078,7 +6073,7 @@
         <v>8063</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -6086,7 +6081,7 @@
         <v>8064</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -6095,7 +6090,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -6104,7 +6099,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -6113,7 +6108,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6122,7 +6117,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -6130,30 +6125,30 @@
         <v>4</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C22" s="35"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C23" s="36"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C25" s="38"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -6161,7 +6156,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>1</v>
@@ -6172,7 +6167,7 @@
         <v>8060</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -6180,7 +6175,7 @@
         <v>8061</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -6188,7 +6183,7 @@
         <v>8062</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -6196,7 +6191,7 @@
         <v>8063</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -6204,7 +6199,7 @@
         <v>8064</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
@@ -6212,7 +6207,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
@@ -6220,7 +6215,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
@@ -6228,7 +6223,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
@@ -6236,7 +6231,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
@@ -6244,7 +6239,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -6279,19 +6274,19 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" s="35"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C3" s="36"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" s="38"/>
     </row>
@@ -6305,7 +6300,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
@@ -6314,7 +6309,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="10">
         <v>31</v>
@@ -6323,7 +6318,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10">
         <v>31</v>
@@ -6332,7 +6327,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="10">
         <v>31</v>
@@ -6341,7 +6336,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="10">
         <v>31</v>
@@ -6350,7 +6345,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="10">
         <v>31</v>
@@ -6359,7 +6354,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="10">
         <v>31</v>
@@ -6377,7 +6372,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="10">
         <v>31</v>
@@ -6386,7 +6381,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" s="10">
         <v>31</v>
@@ -6395,7 +6390,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C17" s="10">
         <v>31</v>
@@ -6413,7 +6408,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="10">
         <v>31</v>
@@ -6421,7 +6416,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C20" s="10">
         <v>30</v>
@@ -6429,7 +6424,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="10">
         <v>30</v>
@@ -6437,7 +6432,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C22" s="10">
         <v>30</v>
@@ -6445,7 +6440,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C23" s="10">
         <v>28</v>
@@ -6453,7 +6448,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C24" s="10">
         <v>30</v>
@@ -6461,7 +6456,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C25" s="10">
         <v>28</v>
@@ -6509,7 +6504,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C31" s="10">
         <v>30</v>
@@ -6528,10 +6523,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:D69"/>
+  <dimension ref="B2:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6543,7 +6538,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="35"/>
     </row>
@@ -6577,10 +6572,10 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
@@ -6588,7 +6583,7 @@
         <v>36892</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
@@ -6596,7 +6591,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
@@ -6604,47 +6599,47 @@
         <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -6652,7 +6647,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -6660,7 +6655,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -6668,39 +6663,39 @@
         <v>1.25</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
@@ -6708,7 +6703,7 @@
         <v>0.61284722222222221</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -6716,7 +6711,7 @@
         <v>0.61249999999999993</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -6724,7 +6719,7 @@
         <v>0.83332175925925922</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -6732,19 +6727,19 @@
         <v>0.1125</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="36" t="s">
-        <v>15</v>
+        <v>184</v>
       </c>
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
@@ -6761,7 +6756,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>0</v>
@@ -6772,7 +6767,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>1</v>
@@ -6780,86 +6775,86 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -6868,165 +6863,163 @@
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="11" t="s">
-        <v>20</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>48</v>
+        <v>26</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="9" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>128</v>
+      <c r="B52" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="11" t="s">
-        <v>26</v>
+      <c r="B53" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>130</v>
+        <v>33</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="11" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>132</v>
+        <v>33</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="11" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="34">
+      <c r="B58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" s="34">
         <v>1.25</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="C59" s="10" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="25" t="s">
-        <v>100</v>
+      <c r="B60" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>133</v>
@@ -7034,90 +7027,101 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>179</v>
+        <v>33</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="26">
-        <v>0.61284722222222221</v>
+      <c r="B63" s="25" t="s">
+        <v>100</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="26">
-        <v>0.61249999999999993</v>
+        <v>0.61284722222222221</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="26">
-        <v>0.83332175925925922</v>
+        <v>0.61249999999999993</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="27">
+      <c r="B66" s="26">
+        <v>0.83332175925925922</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="27">
         <v>0.1125</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>49</v>
+      <c r="C67" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C69" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>50</v>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -7130,6 +7134,7 @@
     <mergeCell ref="B32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-4494 bug fix; Number of month of all dates methods should start from 1
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Date.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Date.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="762" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="7" r:id="rId1"/>
@@ -1969,6 +1969,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1984,13 +1994,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2011,10 +2015,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2407,85 +2407,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="F2" s="72" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="F2" s="76" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="J2" s="72" t="s">
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="J2" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="N2" s="72" t="s">
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="N2" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="R2" s="72" t="s">
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="R2" s="76" t="s">
         <v>174</v>
       </c>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="F3" s="73" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="F3" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="J3" s="73" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="N3" s="73" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="N3" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="R3" s="73" t="s">
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="R3" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-      <c r="F5" s="77" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="F5" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="J5" s="74" t="s">
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
+      <c r="J5" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="75"/>
-      <c r="L5" s="76"/>
-      <c r="N5" s="74" t="s">
+      <c r="K5" s="79"/>
+      <c r="L5" s="80"/>
+      <c r="N5" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="O5" s="75"/>
-      <c r="P5" s="76"/>
-      <c r="R5" s="74" t="s">
+      <c r="O5" s="79"/>
+      <c r="P5" s="80"/>
+      <c r="R5" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="S5" s="75"/>
-      <c r="T5" s="76"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="80"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -5301,12 +5301,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="N5:P5"/>
@@ -5316,6 +5310,12 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="N3:P3"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5327,8 +5327,8 @@
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5343,55 +5343,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="F2" s="72" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="F2" s="76" t="s">
         <v>179</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="J2" s="72" t="s">
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="J2" s="76" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="F3" s="73" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="F3" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="J3" s="73" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-      <c r="F5" s="77" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="F5" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="J5" s="77" t="s">
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
+      <c r="J5" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="79"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="75"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -5483,7 +5483,7 @@
         <v>67</v>
       </c>
       <c r="H9" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J9" s="25"/>
       <c r="K9" s="10" t="s">
@@ -5507,7 +5507,7 @@
         <v>68</v>
       </c>
       <c r="H10" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="10" t="s">
@@ -5531,7 +5531,7 @@
         <v>69</v>
       </c>
       <c r="H11" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="10" t="s">
@@ -5554,7 +5554,7 @@
         <v>70</v>
       </c>
       <c r="H12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="10" t="s">
@@ -5577,7 +5577,7 @@
         <v>71</v>
       </c>
       <c r="H13" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="10" t="s">
@@ -5600,7 +5600,7 @@
         <v>72</v>
       </c>
       <c r="H14" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="10" t="s">
@@ -5623,7 +5623,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="4">
@@ -5646,7 +5646,7 @@
         <v>24</v>
       </c>
       <c r="H16" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="5" t="s">
@@ -5669,7 +5669,7 @@
         <v>140</v>
       </c>
       <c r="H17" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" s="25"/>
       <c r="K17" s="5" t="s">
@@ -5692,7 +5692,7 @@
         <v>141</v>
       </c>
       <c r="H18" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="17" t="s">
@@ -5715,7 +5715,7 @@
         <v>1.25</v>
       </c>
       <c r="H19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="25"/>
       <c r="K19" s="22">
@@ -5738,7 +5738,7 @@
         <v>81</v>
       </c>
       <c r="H20" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J20" s="25"/>
       <c r="K20" s="10" t="s">
@@ -5794,85 +5794,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="F2" s="72" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="F2" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="J2" s="72" t="s">
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="J2" s="76" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="N2" s="72" t="s">
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="N2" s="76" t="s">
         <v>184</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="R2" s="72" t="s">
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="R2" s="76" t="s">
         <v>185</v>
       </c>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="F3" s="73" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="F3" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="J3" s="73" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="N3" s="73" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="N3" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="R3" s="73" t="s">
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="R3" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-      <c r="F5" s="77" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="F5" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="J5" s="77" t="s">
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
+      <c r="J5" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="79"/>
-      <c r="N5" s="77" t="s">
+      <c r="K5" s="74"/>
+      <c r="L5" s="75"/>
+      <c r="N5" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="O5" s="78"/>
-      <c r="P5" s="79"/>
-      <c r="R5" s="77" t="s">
+      <c r="O5" s="74"/>
+      <c r="P5" s="75"/>
+      <c r="R5" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="S5" s="78"/>
-      <c r="T5" s="79"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="75"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -6544,25 +6544,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -6675,25 +6675,25 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="76" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="77" t="s">
+      <c r="B24" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="78"/>
-      <c r="D24" s="79"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="75"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="41" t="s">
@@ -6852,8 +6852,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:P220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6873,64 +6873,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="G2" s="72" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="G2" s="76" t="s">
         <v>245</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="L2" s="72" t="s">
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="L2" s="76" t="s">
         <v>293</v>
       </c>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="G3" s="73" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="G3" s="77" t="s">
         <v>251</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="L3" s="73" t="s">
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="L3" s="77" t="s">
         <v>292</v>
       </c>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="79"/>
-      <c r="G5" s="77" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="G5" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="79"/>
-      <c r="L5" s="77" t="s">
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
+      <c r="L5" s="73" t="s">
         <v>334</v>
       </c>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="79"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="75"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -8062,64 +8062,64 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="G44" s="72" t="s">
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="G44" s="76" t="s">
         <v>246</v>
       </c>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="L44" s="72" t="s">
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="L44" s="76" t="s">
         <v>342</v>
       </c>
-      <c r="M44" s="72"/>
-      <c r="N44" s="72"/>
-      <c r="O44" s="72"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="76"/>
     </row>
     <row r="45" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="G45" s="73" t="s">
+      <c r="C45" s="77"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="G45" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="H45" s="73"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="L45" s="73" t="s">
+      <c r="H45" s="77"/>
+      <c r="I45" s="77"/>
+      <c r="J45" s="77"/>
+      <c r="L45" s="77" t="s">
         <v>341</v>
       </c>
-      <c r="M45" s="73"/>
-      <c r="N45" s="73"/>
-      <c r="O45" s="73"/>
+      <c r="M45" s="77"/>
+      <c r="N45" s="77"/>
+      <c r="O45" s="77"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B47" s="77" t="s">
+      <c r="B47" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="79"/>
-      <c r="G47" s="77" t="s">
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="75"/>
+      <c r="G47" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="H47" s="78"/>
-      <c r="I47" s="78"/>
-      <c r="J47" s="79"/>
-      <c r="L47" s="77" t="s">
+      <c r="H47" s="74"/>
+      <c r="I47" s="74"/>
+      <c r="J47" s="75"/>
+      <c r="L47" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="M47" s="78"/>
-      <c r="N47" s="78"/>
-      <c r="O47" s="79"/>
+      <c r="M47" s="74"/>
+      <c r="N47" s="74"/>
+      <c r="O47" s="75"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" s="41" t="s">
@@ -8770,64 +8770,64 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B74" s="72" t="s">
+      <c r="B74" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="C74" s="72"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="72"/>
-      <c r="G74" s="72" t="s">
+      <c r="C74" s="76"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="76"/>
+      <c r="G74" s="76" t="s">
         <v>247</v>
       </c>
-      <c r="H74" s="72"/>
-      <c r="I74" s="72"/>
-      <c r="J74" s="72"/>
-      <c r="L74" s="72" t="s">
+      <c r="H74" s="76"/>
+      <c r="I74" s="76"/>
+      <c r="J74" s="76"/>
+      <c r="L74" s="76" t="s">
         <v>337</v>
       </c>
-      <c r="M74" s="72"/>
-      <c r="N74" s="72"/>
-      <c r="O74" s="72"/>
+      <c r="M74" s="76"/>
+      <c r="N74" s="76"/>
+      <c r="O74" s="76"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="73"/>
-      <c r="D75" s="73"/>
-      <c r="E75" s="73"/>
-      <c r="G75" s="73" t="s">
+      <c r="C75" s="77"/>
+      <c r="D75" s="77"/>
+      <c r="E75" s="77"/>
+      <c r="G75" s="77" t="s">
         <v>253</v>
       </c>
-      <c r="H75" s="73"/>
-      <c r="I75" s="73"/>
-      <c r="J75" s="73"/>
-      <c r="L75" s="73" t="s">
+      <c r="H75" s="77"/>
+      <c r="I75" s="77"/>
+      <c r="J75" s="77"/>
+      <c r="L75" s="77" t="s">
         <v>335</v>
       </c>
-      <c r="M75" s="73"/>
-      <c r="N75" s="73"/>
-      <c r="O75" s="73"/>
+      <c r="M75" s="77"/>
+      <c r="N75" s="77"/>
+      <c r="O75" s="77"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B77" s="77" t="s">
+      <c r="B77" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="C77" s="78"/>
-      <c r="D77" s="78"/>
-      <c r="E77" s="79"/>
-      <c r="G77" s="77" t="s">
+      <c r="C77" s="74"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="75"/>
+      <c r="G77" s="73" t="s">
         <v>191</v>
       </c>
-      <c r="H77" s="78"/>
-      <c r="I77" s="78"/>
-      <c r="J77" s="79"/>
-      <c r="L77" s="77" t="s">
+      <c r="H77" s="74"/>
+      <c r="I77" s="74"/>
+      <c r="J77" s="75"/>
+      <c r="L77" s="73" t="s">
         <v>338</v>
       </c>
-      <c r="M77" s="78"/>
-      <c r="N77" s="78"/>
-      <c r="O77" s="79"/>
+      <c r="M77" s="74"/>
+      <c r="N77" s="74"/>
+      <c r="O77" s="75"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B78" s="41" t="s">
@@ -9701,7 +9701,7 @@
       <c r="N102" s="4">
         <v>42766</v>
       </c>
-      <c r="O102" s="87">
+      <c r="O102" s="72">
         <v>0</v>
       </c>
     </row>
@@ -9739,7 +9739,7 @@
       <c r="N103" s="4">
         <v>43891</v>
       </c>
-      <c r="O103" s="87">
+      <c r="O103" s="72">
         <v>0</v>
       </c>
     </row>
@@ -9934,64 +9934,64 @@
       </c>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B113" s="72" t="s">
+      <c r="B113" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="C113" s="72"/>
-      <c r="D113" s="72"/>
-      <c r="E113" s="72"/>
-      <c r="G113" s="72" t="s">
+      <c r="C113" s="76"/>
+      <c r="D113" s="76"/>
+      <c r="E113" s="76"/>
+      <c r="G113" s="76" t="s">
         <v>248</v>
       </c>
-      <c r="H113" s="72"/>
-      <c r="I113" s="72"/>
-      <c r="J113" s="72"/>
-      <c r="L113" s="72" t="s">
+      <c r="H113" s="76"/>
+      <c r="I113" s="76"/>
+      <c r="J113" s="76"/>
+      <c r="L113" s="76" t="s">
         <v>339</v>
       </c>
-      <c r="M113" s="72"/>
-      <c r="N113" s="72"/>
-      <c r="O113" s="72"/>
+      <c r="M113" s="76"/>
+      <c r="N113" s="76"/>
+      <c r="O113" s="76"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B114" s="73" t="s">
+      <c r="B114" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="C114" s="73"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="73"/>
-      <c r="G114" s="73" t="s">
+      <c r="C114" s="77"/>
+      <c r="D114" s="77"/>
+      <c r="E114" s="77"/>
+      <c r="G114" s="77" t="s">
         <v>254</v>
       </c>
-      <c r="H114" s="73"/>
-      <c r="I114" s="73"/>
-      <c r="J114" s="73"/>
-      <c r="L114" s="73" t="s">
+      <c r="H114" s="77"/>
+      <c r="I114" s="77"/>
+      <c r="J114" s="77"/>
+      <c r="L114" s="77" t="s">
         <v>336</v>
       </c>
-      <c r="M114" s="73"/>
-      <c r="N114" s="73"/>
-      <c r="O114" s="73"/>
+      <c r="M114" s="77"/>
+      <c r="N114" s="77"/>
+      <c r="O114" s="77"/>
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B116" s="77" t="s">
+      <c r="B116" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="C116" s="78"/>
-      <c r="D116" s="78"/>
-      <c r="E116" s="79"/>
-      <c r="G116" s="77" t="s">
+      <c r="C116" s="74"/>
+      <c r="D116" s="74"/>
+      <c r="E116" s="75"/>
+      <c r="G116" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="H116" s="78"/>
-      <c r="I116" s="78"/>
-      <c r="J116" s="79"/>
-      <c r="L116" s="77" t="s">
+      <c r="H116" s="74"/>
+      <c r="I116" s="74"/>
+      <c r="J116" s="75"/>
+      <c r="L116" s="73" t="s">
         <v>340</v>
       </c>
-      <c r="M116" s="78"/>
-      <c r="N116" s="78"/>
-      <c r="O116" s="79"/>
+      <c r="M116" s="74"/>
+      <c r="N116" s="74"/>
+      <c r="O116" s="75"/>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B117" s="41" t="s">
@@ -10666,7 +10666,7 @@
       </c>
       <c r="M135" s="17"/>
       <c r="N135" s="17"/>
-      <c r="O135" s="87">
+      <c r="O135" s="72">
         <v>0</v>
       </c>
     </row>
@@ -10700,7 +10700,7 @@
         <v>67</v>
       </c>
       <c r="N136" s="17"/>
-      <c r="O136" s="87"/>
+      <c r="O136" s="72"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B137" s="49" t="s">
@@ -10732,7 +10732,7 @@
       <c r="N137" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="O137" s="87"/>
+      <c r="O137" s="72"/>
     </row>
     <row r="138" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B138" s="49" t="s">
@@ -10832,7 +10832,7 @@
       <c r="N141" s="4">
         <v>42795</v>
       </c>
-      <c r="O141" s="87">
+      <c r="O141" s="72">
         <v>29</v>
       </c>
     </row>
@@ -10846,33 +10846,33 @@
       <c r="N142" s="48" t="s">
         <v>385</v>
       </c>
-      <c r="O142" s="87">
+      <c r="O142" s="72">
         <v>365</v>
       </c>
     </row>
     <row r="145" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G145" s="72" t="s">
+      <c r="G145" s="76" t="s">
         <v>249</v>
       </c>
-      <c r="H145" s="72"/>
-      <c r="I145" s="72"/>
-      <c r="J145" s="72"/>
+      <c r="H145" s="76"/>
+      <c r="I145" s="76"/>
+      <c r="J145" s="76"/>
     </row>
     <row r="146" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G146" s="73" t="s">
+      <c r="G146" s="77" t="s">
         <v>255</v>
       </c>
-      <c r="H146" s="73"/>
-      <c r="I146" s="73"/>
-      <c r="J146" s="73"/>
+      <c r="H146" s="77"/>
+      <c r="I146" s="77"/>
+      <c r="J146" s="77"/>
     </row>
     <row r="148" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G148" s="77" t="s">
+      <c r="G148" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="H148" s="78"/>
-      <c r="I148" s="78"/>
-      <c r="J148" s="79"/>
+      <c r="H148" s="74"/>
+      <c r="I148" s="74"/>
+      <c r="J148" s="75"/>
     </row>
     <row r="149" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G149" s="41" t="s">
@@ -11059,28 +11059,28 @@
       </c>
     </row>
     <row r="167" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G167" s="72" t="s">
+      <c r="G167" s="76" t="s">
         <v>258</v>
       </c>
-      <c r="H167" s="72"/>
-      <c r="I167" s="72"/>
-      <c r="J167" s="72"/>
+      <c r="H167" s="76"/>
+      <c r="I167" s="76"/>
+      <c r="J167" s="76"/>
     </row>
     <row r="168" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G168" s="73" t="s">
+      <c r="G168" s="77" t="s">
         <v>256</v>
       </c>
-      <c r="H168" s="73"/>
-      <c r="I168" s="73"/>
-      <c r="J168" s="73"/>
+      <c r="H168" s="77"/>
+      <c r="I168" s="77"/>
+      <c r="J168" s="77"/>
     </row>
     <row r="170" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G170" s="77" t="s">
+      <c r="G170" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="H170" s="78"/>
-      <c r="I170" s="78"/>
-      <c r="J170" s="79"/>
+      <c r="H170" s="74"/>
+      <c r="I170" s="74"/>
+      <c r="J170" s="75"/>
     </row>
     <row r="171" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G171" s="41" t="s">
@@ -11351,28 +11351,28 @@
       </c>
     </row>
     <row r="196" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G196" s="80" t="s">
+      <c r="G196" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="H196" s="81"/>
-      <c r="I196" s="81"/>
-      <c r="J196" s="82"/>
+      <c r="H196" s="83"/>
+      <c r="I196" s="83"/>
+      <c r="J196" s="84"/>
     </row>
     <row r="197" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G197" s="83" t="s">
+      <c r="G197" s="85" t="s">
         <v>257</v>
       </c>
-      <c r="H197" s="84"/>
-      <c r="I197" s="84"/>
-      <c r="J197" s="85"/>
+      <c r="H197" s="86"/>
+      <c r="I197" s="86"/>
+      <c r="J197" s="87"/>
     </row>
     <row r="199" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G199" s="77" t="s">
+      <c r="G199" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="H199" s="78"/>
-      <c r="I199" s="78"/>
-      <c r="J199" s="86"/>
+      <c r="H199" s="74"/>
+      <c r="I199" s="74"/>
+      <c r="J199" s="81"/>
     </row>
     <row r="200" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G200" s="41" t="s">
@@ -11620,12 +11620,29 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B116:E116"/>
-    <mergeCell ref="G114:J114"/>
-    <mergeCell ref="G77:J77"/>
-    <mergeCell ref="G145:J145"/>
-    <mergeCell ref="G146:J146"/>
-    <mergeCell ref="G113:J113"/>
+    <mergeCell ref="L113:O113"/>
+    <mergeCell ref="L114:O114"/>
+    <mergeCell ref="L45:O45"/>
+    <mergeCell ref="L47:O47"/>
+    <mergeCell ref="L77:O77"/>
+    <mergeCell ref="L74:O74"/>
+    <mergeCell ref="L75:O75"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="G196:J196"/>
+    <mergeCell ref="G197:J197"/>
+    <mergeCell ref="G148:J148"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G74:J74"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G75:J75"/>
+    <mergeCell ref="L116:O116"/>
+    <mergeCell ref="L44:O44"/>
     <mergeCell ref="G199:J199"/>
     <mergeCell ref="G116:J116"/>
     <mergeCell ref="B2:E2"/>
@@ -11642,29 +11659,12 @@
     <mergeCell ref="G168:J168"/>
     <mergeCell ref="G170:J170"/>
     <mergeCell ref="B114:E114"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="G196:J196"/>
-    <mergeCell ref="G197:J197"/>
-    <mergeCell ref="G148:J148"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="G45:J45"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G74:J74"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G75:J75"/>
-    <mergeCell ref="L116:O116"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="L113:O113"/>
-    <mergeCell ref="L114:O114"/>
-    <mergeCell ref="L45:O45"/>
-    <mergeCell ref="L47:O47"/>
-    <mergeCell ref="L77:O77"/>
-    <mergeCell ref="L74:O74"/>
-    <mergeCell ref="L75:O75"/>
+    <mergeCell ref="B116:E116"/>
+    <mergeCell ref="G114:J114"/>
+    <mergeCell ref="G77:J77"/>
+    <mergeCell ref="G145:J145"/>
+    <mergeCell ref="G146:J146"/>
+    <mergeCell ref="G113:J113"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -11689,25 +11689,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
@@ -11830,25 +11830,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="76" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="78"/>
-      <c r="D25" s="79"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="75"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="53" t="s">
@@ -11994,25 +11994,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -12298,25 +12298,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -12528,28 +12528,28 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="C33" s="73"/>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="79"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="75"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="41" t="s">

</xml_diff>

<commit_message>
EPBDS-7572 The difference between two date cannot be calculated if both dates are unknown
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Date.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Date.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="7" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="P84" authorId="0" shapeId="0">
+    <comment ref="P84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +62,7 @@
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="L23" authorId="0" shapeId="0">
+    <comment ref="L23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L24" authorId="0" shapeId="0">
+    <comment ref="L24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +125,7 @@
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="D31" authorId="0" shapeId="0">
+    <comment ref="D31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +168,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +231,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="E71" authorId="0" shapeId="0">
+    <comment ref="E71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -840,7 +835,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
@@ -1116,34 +1111,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1154,9 +1125,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1546,190 +1541,190 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="F2" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="N2" s="37" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="R2" s="37" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="R2" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="F3" s="38" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="F3" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="J3" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="N3" s="38" t="s">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="R3" s="38" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="R3" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="F5" s="35" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="F5" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="36"/>
-      <c r="J5" s="44" t="s">
+      <c r="G5" s="55"/>
+      <c r="H5" s="56"/>
+      <c r="J5" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="46"/>
-      <c r="N5" s="44" t="s">
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
+      <c r="N5" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="O5" s="45"/>
-      <c r="P5" s="46"/>
-      <c r="R5" s="44" t="s">
+      <c r="O5" s="52"/>
+      <c r="P5" s="53"/>
+      <c r="R5" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="S5" s="45"/>
-      <c r="T5" s="46"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="53"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="K6" s="48" t="s">
+      <c r="K6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="49" t="s">
+      <c r="P6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="S6" s="48" t="s">
+      <c r="S6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="49" t="s">
+      <c r="T6" s="41" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="54" t="s">
+      <c r="D7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="54" t="s">
+      <c r="H7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="K7" s="55" t="s">
+      <c r="K7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="54" t="s">
+      <c r="L7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="O7" s="55" t="s">
+      <c r="O7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" s="54" t="s">
+      <c r="P7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="S7" s="55" t="s">
+      <c r="S7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="T7" s="42" t="s">
+      <c r="T7" s="37" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
       <c r="F8" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="G8" s="43"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="26"/>
       <c r="J8" s="26" t="s">
         <v>177</v>
@@ -1756,7 +1751,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="26"/>
-      <c r="G9" s="43">
+      <c r="G9" s="38">
         <v>42197</v>
       </c>
       <c r="H9" s="10">
@@ -1793,7 +1788,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="43">
+      <c r="G10" s="38">
         <v>42197.000011574077</v>
       </c>
       <c r="H10" s="10">
@@ -1830,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="43">
+      <c r="G11" s="38">
         <v>42197.041655092595</v>
       </c>
       <c r="H11" s="17">
@@ -1867,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="43">
+      <c r="G12" s="38">
         <v>42197.041666666664</v>
       </c>
       <c r="H12" s="10">
@@ -1904,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="26"/>
-      <c r="G13" s="43">
+      <c r="G13" s="38">
         <v>42197.041678240741</v>
       </c>
       <c r="H13" s="10">
@@ -1941,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="26"/>
-      <c r="G14" s="43">
+      <c r="G14" s="38">
         <v>42197.083321759259</v>
       </c>
       <c r="H14" s="17">
@@ -1978,7 +1973,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="26"/>
-      <c r="G15" s="43">
+      <c r="G15" s="38">
         <v>42197.083333333328</v>
       </c>
       <c r="H15" s="10">
@@ -2015,7 +2010,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="26"/>
-      <c r="G16" s="43">
+      <c r="G16" s="38">
         <v>42197.083344907405</v>
       </c>
       <c r="H16" s="10">
@@ -2052,7 +2047,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="26"/>
-      <c r="G17" s="43">
+      <c r="G17" s="38">
         <v>42197.124988425923</v>
       </c>
       <c r="H17" s="17">
@@ -2089,7 +2084,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="43">
+      <c r="G18" s="38">
         <v>42197.124999999993</v>
       </c>
       <c r="H18" s="10">
@@ -2126,7 +2121,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="26"/>
-      <c r="G19" s="43">
+      <c r="G19" s="38">
         <v>42197.12501157407</v>
       </c>
       <c r="H19" s="10">
@@ -2163,7 +2158,7 @@
         <v>10</v>
       </c>
       <c r="F20" s="26"/>
-      <c r="G20" s="43">
+      <c r="G20" s="38">
         <v>42197.166655092587</v>
       </c>
       <c r="H20" s="17">
@@ -2200,7 +2195,7 @@
         <v>10</v>
       </c>
       <c r="F21" s="26"/>
-      <c r="G21" s="43">
+      <c r="G21" s="38">
         <v>42197.166666666657</v>
       </c>
       <c r="H21" s="10">
@@ -2237,7 +2232,7 @@
         <v>10</v>
       </c>
       <c r="F22" s="26"/>
-      <c r="G22" s="43">
+      <c r="G22" s="38">
         <v>42197.166678240734</v>
       </c>
       <c r="H22" s="10">
@@ -2274,7 +2269,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="26"/>
-      <c r="G23" s="43">
+      <c r="G23" s="38">
         <v>42197.208321759252</v>
       </c>
       <c r="H23" s="17">
@@ -2311,7 +2306,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="26"/>
-      <c r="G24" s="43">
+      <c r="G24" s="38">
         <v>42197.208333333321</v>
       </c>
       <c r="H24" s="10">
@@ -2348,7 +2343,7 @@
         <v>10</v>
       </c>
       <c r="F25" s="26"/>
-      <c r="G25" s="43">
+      <c r="G25" s="38">
         <v>42197.208344907398</v>
       </c>
       <c r="H25" s="10">
@@ -2385,7 +2380,7 @@
         <v>10</v>
       </c>
       <c r="F26" s="26"/>
-      <c r="G26" s="43">
+      <c r="G26" s="38">
         <v>42197.249988425916</v>
       </c>
       <c r="H26" s="17">
@@ -2422,7 +2417,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="26"/>
-      <c r="G27" s="43">
+      <c r="G27" s="38">
         <v>42197.249999999985</v>
       </c>
       <c r="H27" s="10">
@@ -2459,7 +2454,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="26"/>
-      <c r="G28" s="43">
+      <c r="G28" s="38">
         <v>42197.250011574062</v>
       </c>
       <c r="H28" s="10">
@@ -2496,7 +2491,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="26"/>
-      <c r="G29" s="43">
+      <c r="G29" s="38">
         <v>42197.29165509258</v>
       </c>
       <c r="H29" s="17">
@@ -2533,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="F30" s="26"/>
-      <c r="G30" s="43">
+      <c r="G30" s="38">
         <v>42197.29166666665</v>
       </c>
       <c r="H30" s="10">
@@ -2570,7 +2565,7 @@
         <v>10</v>
       </c>
       <c r="F31" s="26"/>
-      <c r="G31" s="43">
+      <c r="G31" s="38">
         <v>42197.291678240726</v>
       </c>
       <c r="H31" s="10">
@@ -2607,7 +2602,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="26"/>
-      <c r="G32" s="43">
+      <c r="G32" s="38">
         <v>42197.333321759244</v>
       </c>
       <c r="H32" s="17">
@@ -2644,7 +2639,7 @@
         <v>10</v>
       </c>
       <c r="F33" s="26"/>
-      <c r="G33" s="43">
+      <c r="G33" s="38">
         <v>42197.333333333314</v>
       </c>
       <c r="H33" s="10">
@@ -2681,7 +2676,7 @@
         <v>10</v>
       </c>
       <c r="F34" s="26"/>
-      <c r="G34" s="43">
+      <c r="G34" s="38">
         <v>42197.333344907391</v>
       </c>
       <c r="H34" s="10">
@@ -2718,7 +2713,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="26"/>
-      <c r="G35" s="43">
+      <c r="G35" s="38">
         <v>42197.374988425909</v>
       </c>
       <c r="H35" s="17">
@@ -2755,7 +2750,7 @@
         <v>10</v>
       </c>
       <c r="F36" s="26"/>
-      <c r="G36" s="43">
+      <c r="G36" s="38">
         <v>42197.374999999978</v>
       </c>
       <c r="H36" s="10">
@@ -2792,7 +2787,7 @@
         <v>10</v>
       </c>
       <c r="F37" s="26"/>
-      <c r="G37" s="43">
+      <c r="G37" s="38">
         <v>42197.375011574055</v>
       </c>
       <c r="H37" s="10">
@@ -2829,7 +2824,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="26"/>
-      <c r="G38" s="43">
+      <c r="G38" s="38">
         <v>42197.416655092573</v>
       </c>
       <c r="H38" s="17">
@@ -2866,7 +2861,7 @@
         <v>10</v>
       </c>
       <c r="F39" s="26"/>
-      <c r="G39" s="43">
+      <c r="G39" s="38">
         <v>42197.416666666642</v>
       </c>
       <c r="H39" s="10">
@@ -2903,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="F40" s="26"/>
-      <c r="G40" s="43">
+      <c r="G40" s="38">
         <v>42197.416678240719</v>
       </c>
       <c r="H40" s="10">
@@ -2940,7 +2935,7 @@
         <v>10</v>
       </c>
       <c r="F41" s="26"/>
-      <c r="G41" s="43">
+      <c r="G41" s="38">
         <v>42197.458321759237</v>
       </c>
       <c r="H41" s="17">
@@ -2977,7 +2972,7 @@
         <v>10</v>
       </c>
       <c r="F42" s="26"/>
-      <c r="G42" s="43">
+      <c r="G42" s="38">
         <v>42197.458333333307</v>
       </c>
       <c r="H42" s="10">
@@ -3014,7 +3009,7 @@
         <v>10</v>
       </c>
       <c r="F43" s="26"/>
-      <c r="G43" s="43">
+      <c r="G43" s="38">
         <v>42197.458344907383</v>
       </c>
       <c r="H43" s="10">
@@ -3051,7 +3046,7 @@
         <v>10</v>
       </c>
       <c r="F44" s="26"/>
-      <c r="G44" s="43">
+      <c r="G44" s="38">
         <v>42197.499988425901</v>
       </c>
       <c r="H44" s="17">
@@ -3088,7 +3083,7 @@
         <v>127</v>
       </c>
       <c r="F45" s="26"/>
-      <c r="G45" s="43">
+      <c r="G45" s="38">
         <v>42197.499999999971</v>
       </c>
       <c r="H45" s="10">
@@ -3125,7 +3120,7 @@
         <v>127</v>
       </c>
       <c r="F46" s="26"/>
-      <c r="G46" s="43">
+      <c r="G46" s="38">
         <v>42197.500011574048</v>
       </c>
       <c r="H46" s="10">
@@ -3162,7 +3157,7 @@
         <v>127</v>
       </c>
       <c r="F47" s="26"/>
-      <c r="G47" s="43">
+      <c r="G47" s="38">
         <v>42197.541655092566</v>
       </c>
       <c r="H47" s="17">
@@ -3199,7 +3194,7 @@
         <v>127</v>
       </c>
       <c r="F48" s="26"/>
-      <c r="G48" s="43">
+      <c r="G48" s="38">
         <v>42197.541666666635</v>
       </c>
       <c r="H48" s="10">
@@ -3236,7 +3231,7 @@
         <v>127</v>
       </c>
       <c r="F49" s="26"/>
-      <c r="G49" s="43">
+      <c r="G49" s="38">
         <v>42197.541678240712</v>
       </c>
       <c r="H49" s="10">
@@ -3273,7 +3268,7 @@
         <v>127</v>
       </c>
       <c r="F50" s="26"/>
-      <c r="G50" s="43">
+      <c r="G50" s="38">
         <v>42197.58332175923</v>
       </c>
       <c r="H50" s="17">
@@ -3310,7 +3305,7 @@
         <v>127</v>
       </c>
       <c r="F51" s="26"/>
-      <c r="G51" s="43">
+      <c r="G51" s="38">
         <v>42197.583333333299</v>
       </c>
       <c r="H51" s="10">
@@ -3347,7 +3342,7 @@
         <v>127</v>
       </c>
       <c r="F52" s="26"/>
-      <c r="G52" s="43">
+      <c r="G52" s="38">
         <v>42197.583344907376</v>
       </c>
       <c r="H52" s="10">
@@ -3384,7 +3379,7 @@
         <v>127</v>
       </c>
       <c r="F53" s="26"/>
-      <c r="G53" s="43">
+      <c r="G53" s="38">
         <v>42197.624988425894</v>
       </c>
       <c r="H53" s="17">
@@ -3421,7 +3416,7 @@
         <v>127</v>
       </c>
       <c r="F54" s="26"/>
-      <c r="G54" s="43">
+      <c r="G54" s="38">
         <v>42197.624999999964</v>
       </c>
       <c r="H54" s="10">
@@ -3458,7 +3453,7 @@
         <v>127</v>
       </c>
       <c r="F55" s="26"/>
-      <c r="G55" s="43">
+      <c r="G55" s="38">
         <v>42197.62501157404</v>
       </c>
       <c r="H55" s="10">
@@ -3495,7 +3490,7 @@
         <v>127</v>
       </c>
       <c r="F56" s="26"/>
-      <c r="G56" s="43">
+      <c r="G56" s="38">
         <v>42197.666655092558</v>
       </c>
       <c r="H56" s="17">
@@ -3532,7 +3527,7 @@
         <v>127</v>
       </c>
       <c r="F57" s="26"/>
-      <c r="G57" s="43">
+      <c r="G57" s="38">
         <v>42197.666666666628</v>
       </c>
       <c r="H57" s="10">
@@ -3569,7 +3564,7 @@
         <v>127</v>
       </c>
       <c r="F58" s="26"/>
-      <c r="G58" s="43">
+      <c r="G58" s="38">
         <v>42197.666678240705</v>
       </c>
       <c r="H58" s="10">
@@ -3606,7 +3601,7 @@
         <v>127</v>
       </c>
       <c r="F59" s="26"/>
-      <c r="G59" s="43">
+      <c r="G59" s="38">
         <v>42197.708321759223</v>
       </c>
       <c r="H59" s="17">
@@ -3643,7 +3638,7 @@
         <v>127</v>
       </c>
       <c r="F60" s="26"/>
-      <c r="G60" s="43">
+      <c r="G60" s="38">
         <v>42197.708333333292</v>
       </c>
       <c r="H60" s="10">
@@ -3680,7 +3675,7 @@
         <v>127</v>
       </c>
       <c r="F61" s="26"/>
-      <c r="G61" s="43">
+      <c r="G61" s="38">
         <v>42197.708344907369</v>
       </c>
       <c r="H61" s="10">
@@ -3717,7 +3712,7 @@
         <v>127</v>
       </c>
       <c r="F62" s="26"/>
-      <c r="G62" s="43">
+      <c r="G62" s="38">
         <v>42197.749988425887</v>
       </c>
       <c r="H62" s="17">
@@ -3754,7 +3749,7 @@
         <v>127</v>
       </c>
       <c r="F63" s="26"/>
-      <c r="G63" s="43">
+      <c r="G63" s="38">
         <v>42197.749999999956</v>
       </c>
       <c r="H63" s="10">
@@ -3791,7 +3786,7 @@
         <v>127</v>
       </c>
       <c r="F64" s="26"/>
-      <c r="G64" s="43">
+      <c r="G64" s="38">
         <v>42197.750011574033</v>
       </c>
       <c r="H64" s="10">
@@ -3828,7 +3823,7 @@
         <v>127</v>
       </c>
       <c r="F65" s="26"/>
-      <c r="G65" s="43">
+      <c r="G65" s="38">
         <v>42197.791655092551</v>
       </c>
       <c r="H65" s="17">
@@ -3865,7 +3860,7 @@
         <v>127</v>
       </c>
       <c r="F66" s="26"/>
-      <c r="G66" s="43">
+      <c r="G66" s="38">
         <v>42197.791666666621</v>
       </c>
       <c r="H66" s="10">
@@ -3902,7 +3897,7 @@
         <v>127</v>
       </c>
       <c r="F67" s="26"/>
-      <c r="G67" s="43">
+      <c r="G67" s="38">
         <v>42197.791678240697</v>
       </c>
       <c r="H67" s="10">
@@ -3939,7 +3934,7 @@
         <v>127</v>
       </c>
       <c r="F68" s="26"/>
-      <c r="G68" s="43">
+      <c r="G68" s="38">
         <v>42197.833321759215</v>
       </c>
       <c r="H68" s="17">
@@ -3976,7 +3971,7 @@
         <v>127</v>
       </c>
       <c r="F69" s="26"/>
-      <c r="G69" s="43">
+      <c r="G69" s="38">
         <v>42197.833333333285</v>
       </c>
       <c r="H69" s="10">
@@ -4013,7 +4008,7 @@
         <v>127</v>
       </c>
       <c r="F70" s="26"/>
-      <c r="G70" s="43">
+      <c r="G70" s="38">
         <v>42197.833344907362</v>
       </c>
       <c r="H70" s="10">
@@ -4050,7 +4045,7 @@
         <v>127</v>
       </c>
       <c r="F71" s="26"/>
-      <c r="G71" s="43">
+      <c r="G71" s="38">
         <v>42197.87498842588</v>
       </c>
       <c r="H71" s="17">
@@ -4087,7 +4082,7 @@
         <v>127</v>
       </c>
       <c r="F72" s="26"/>
-      <c r="G72" s="43">
+      <c r="G72" s="38">
         <v>42197.874999999949</v>
       </c>
       <c r="H72" s="10">
@@ -4124,7 +4119,7 @@
         <v>127</v>
       </c>
       <c r="F73" s="26"/>
-      <c r="G73" s="43">
+      <c r="G73" s="38">
         <v>42197.875011574026</v>
       </c>
       <c r="H73" s="10">
@@ -4161,7 +4156,7 @@
         <v>127</v>
       </c>
       <c r="F74" s="26"/>
-      <c r="G74" s="43">
+      <c r="G74" s="38">
         <v>42197.916655092544</v>
       </c>
       <c r="H74" s="17">
@@ -4198,7 +4193,7 @@
         <v>127</v>
       </c>
       <c r="F75" s="26"/>
-      <c r="G75" s="43">
+      <c r="G75" s="38">
         <v>42197.916666666613</v>
       </c>
       <c r="H75" s="10">
@@ -4235,7 +4230,7 @@
         <v>127</v>
       </c>
       <c r="F76" s="26"/>
-      <c r="G76" s="43">
+      <c r="G76" s="38">
         <v>42197.91667824069</v>
       </c>
       <c r="H76" s="10">
@@ -4272,7 +4267,7 @@
         <v>127</v>
       </c>
       <c r="F77" s="26"/>
-      <c r="G77" s="43">
+      <c r="G77" s="38">
         <v>42197.958321759208</v>
       </c>
       <c r="H77" s="17">
@@ -4309,7 +4304,7 @@
         <v>127</v>
       </c>
       <c r="F78" s="26"/>
-      <c r="G78" s="43">
+      <c r="G78" s="38">
         <v>42197.958333333278</v>
       </c>
       <c r="H78" s="10">
@@ -4346,7 +4341,7 @@
         <v>127</v>
       </c>
       <c r="F79" s="26"/>
-      <c r="G79" s="43">
+      <c r="G79" s="38">
         <v>42197.958344907354</v>
       </c>
       <c r="H79" s="10">
@@ -4383,7 +4378,7 @@
         <v>127</v>
       </c>
       <c r="F80" s="26"/>
-      <c r="G80" s="43">
+      <c r="G80" s="38">
         <v>42197.999988425872</v>
       </c>
       <c r="H80" s="17">
@@ -4440,6 +4435,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="N5:P5"/>
@@ -4449,12 +4450,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4482,127 +4477,127 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="F2" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="F3" s="38" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="F3" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="J3" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="F5" s="35" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="F5" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="36"/>
-      <c r="J5" s="35" t="s">
+      <c r="G5" s="55"/>
+      <c r="H5" s="56"/>
+      <c r="J5" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="36"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="56"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="52" t="s">
+      <c r="L6" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="54" t="s">
+      <c r="D7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="54" t="s">
+      <c r="H7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="K7" s="55" t="s">
+      <c r="K7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="37" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="F8" s="53" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="F8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="J8" s="53" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="J8" s="45" t="s">
         <v>177</v>
       </c>
       <c r="K8" s="26"/>
@@ -4933,144 +4928,144 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="F2" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="N2" s="37" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="R2" s="37" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="R2" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="F3" s="38" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="F3" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="J3" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="N3" s="38" t="s">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="R3" s="38" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="R3" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="F5" s="35" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="F5" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="36"/>
-      <c r="J5" s="35" t="s">
+      <c r="G5" s="55"/>
+      <c r="H5" s="56"/>
+      <c r="J5" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="36"/>
-      <c r="N5" s="35" t="s">
+      <c r="K5" s="55"/>
+      <c r="L5" s="56"/>
+      <c r="N5" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="O5" s="39"/>
-      <c r="P5" s="36"/>
-      <c r="R5" s="35" t="s">
+      <c r="O5" s="55"/>
+      <c r="P5" s="56"/>
+      <c r="R5" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="S5" s="39"/>
-      <c r="T5" s="36"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="56"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="52" t="s">
+      <c r="L6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="O6" s="51" t="s">
+      <c r="O6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="52" t="s">
+      <c r="P6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="50" t="s">
+      <c r="R6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="S6" s="51" t="s">
+      <c r="S6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="52" t="s">
+      <c r="T6" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="54" t="s">
+      <c r="D7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>176</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -5079,7 +5074,7 @@
       <c r="H7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="46" t="s">
         <v>176</v>
       </c>
       <c r="K7" s="3" t="s">
@@ -5088,7 +5083,7 @@
       <c r="L7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="54" t="s">
+      <c r="N7" s="46" t="s">
         <v>176</v>
       </c>
       <c r="O7" s="3" t="s">
@@ -5097,7 +5092,7 @@
       <c r="P7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R7" s="54" t="s">
+      <c r="R7" s="46" t="s">
         <v>176</v>
       </c>
       <c r="S7" s="3" t="s">
@@ -5108,31 +5103,31 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="F8" s="53" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="F8" s="45" t="s">
         <v>177</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="45" t="s">
         <v>177</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
-      <c r="N8" s="53" t="s">
+      <c r="N8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="R8" s="53" t="s">
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="R8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
@@ -5195,14 +5190,14 @@
       <c r="L10" s="10">
         <v>5</v>
       </c>
-      <c r="N10" s="53"/>
+      <c r="N10" s="45"/>
       <c r="O10" s="11" t="s">
         <v>68</v>
       </c>
       <c r="P10" s="10">
         <v>1</v>
       </c>
-      <c r="R10" s="53"/>
+      <c r="R10" s="45"/>
       <c r="S10" s="11" t="s">
         <v>68</v>
       </c>
@@ -5682,45 +5677,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="37" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5728,8 +5723,8 @@
       <c r="B8" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
@@ -5813,54 +5808,54 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="36"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="52" t="s">
+      <c r="D25" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C26" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="37" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6"/>
@@ -5988,10 +5983,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="B2:D91"/>
+  <dimension ref="B2:E87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6002,28 +5997,28 @@
     <col min="5" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="36"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -6033,8 +6028,9 @@
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -6045,7 +6041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
@@ -6056,28 +6052,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
         <v>36892</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="7">
         <v>0</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>1</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
@@ -6088,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
         <v>69</v>
       </c>
@@ -6099,7 +6095,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="10">
         <v>2</v>
       </c>
@@ -6110,7 +6106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
         <v>71</v>
       </c>
@@ -6121,7 +6117,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>80</v>
       </c>
@@ -6134,52 +6130,56 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="20">
-        <v>0</v>
-      </c>
+      <c r="C17" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="19" t="s">
         <v>67</v>
       </c>
+      <c r="C18" s="19"/>
       <c r="D18" s="20"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="10">
+        <v>-32872</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="D20" s="10">
-        <v>-32872</v>
+        <v>32872</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>72</v>
+      <c r="B21" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="24">
+        <v>1</v>
       </c>
       <c r="D21" s="10">
-        <v>32872</v>
+        <v>-2016</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="23">
         <v>1</v>
       </c>
       <c r="D22" s="10">
@@ -6188,271 +6188,275 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="10">
         <v>-2016</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="23">
-        <v>2</v>
+      <c r="B24" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>-2016</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="18">
-        <v>1.25</v>
-      </c>
-      <c r="C25" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="55"/>
+      <c r="D31" s="56"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="36"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="B33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="10">
         <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D35" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="10">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1</v>
+      </c>
+      <c r="D36" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="10">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="10">
         <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="10">
-        <v>2</v>
-      </c>
-      <c r="C37" s="10">
-        <v>1</v>
-      </c>
-      <c r="D37" s="10">
-        <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="10">
-        <v>52</v>
+        <v>68</v>
+      </c>
+      <c r="D38" s="21">
+        <v>11270</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="21">
-        <v>11270</v>
-      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="20"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="20">
-        <v>0</v>
-      </c>
+      <c r="B40" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="18"/>
-      <c r="C41" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="20"/>
+      <c r="B41" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="10">
+        <v>-4696</v>
+      </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
+      <c r="B42" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="10">
+        <v>4696</v>
+      </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>79</v>
+      <c r="B43" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="24">
+        <v>1</v>
       </c>
       <c r="D43" s="10">
-        <v>-4696</v>
+        <v>-288</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>72</v>
+      <c r="B44" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="23">
+        <v>1</v>
       </c>
       <c r="D44" s="10">
-        <v>4696</v>
+        <v>-288</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="24">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="C45" s="23">
+        <v>2</v>
       </c>
       <c r="D45" s="10">
         <v>-288</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="23">
-        <v>1</v>
+      <c r="B46" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="C46" s="18">
+        <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>-288</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="55"/>
+      <c r="D53" s="56"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="10">
         <v>2</v>
       </c>
-      <c r="D47" s="10">
-        <v>-288</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="18">
-        <v>1.25</v>
-      </c>
-      <c r="C48" s="18">
-        <v>0</v>
-      </c>
-      <c r="D48" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="36"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>67</v>
+      <c r="C58" s="10">
+        <v>1</v>
       </c>
       <c r="D58" s="10">
         <v>0</v>
@@ -6460,184 +6464,188 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D59" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="10">
+      <c r="B60" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" s="21">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" s="18"/>
+      <c r="C61" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D61" s="20"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="19"/>
+      <c r="D62" s="20"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="20">
+        <v>-1080</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="20">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="24">
+        <v>1</v>
+      </c>
+      <c r="D65" s="20">
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="23">
+        <v>1</v>
+      </c>
+      <c r="D66" s="20">
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="23">
         <v>2</v>
       </c>
-      <c r="C60" s="10">
-        <v>1</v>
-      </c>
-      <c r="D60" s="10">
+      <c r="D67" s="20">
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="C68" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D62" s="21">
-        <v>2591</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="20">
+      <c r="D68" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="18"/>
-      <c r="C64" s="19" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="50"/>
+      <c r="D73" s="50"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" s="55"/>
+      <c r="D75" s="56"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D64" s="20"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="19" t="s">
+      <c r="C78" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="20"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" s="20">
-        <v>-1080</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D67" s="20">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="24">
-        <v>1</v>
-      </c>
-      <c r="D68" s="20">
-        <v>-66</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" s="23">
-        <v>1</v>
-      </c>
-      <c r="D69" s="20">
-        <v>-66</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C70" s="23">
+      <c r="D78" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B79" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B80" s="10">
         <v>2</v>
       </c>
-      <c r="D70" s="20">
-        <v>-66</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B71" s="18">
-        <v>1.25</v>
-      </c>
-      <c r="C71" s="18">
+      <c r="C80" s="10">
+        <v>1</v>
+      </c>
+      <c r="D80" s="10">
         <v>0</v>
-      </c>
-      <c r="D71" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="38"/>
-      <c r="D76" s="38"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B78" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C78" s="39"/>
-      <c r="D78" s="36"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B79" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B80" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D81" s="10">
         <v>0</v>
@@ -6645,116 +6653,76 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="11" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D82" s="10">
-        <v>1</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B83" s="10">
-        <v>2</v>
-      </c>
-      <c r="C83" s="10">
-        <v>1</v>
-      </c>
-      <c r="D83" s="10">
-        <v>0</v>
-      </c>
+      <c r="B83" s="18"/>
+      <c r="C83" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D83" s="20"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B84" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D84" s="10">
-        <v>0</v>
-      </c>
+      <c r="B84" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84" s="19"/>
+      <c r="D84" s="20"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="11" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D85" s="10">
-        <v>215</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="20">
+      <c r="B86" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D86" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B87" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="C87" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B87" s="18"/>
-      <c r="C87" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D87" s="20"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B88" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C88" s="19"/>
-      <c r="D88" s="20"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B89" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D89" s="10">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B90" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D90" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B91" s="18">
-        <v>1.25</v>
-      </c>
-      <c r="C91" s="18">
-        <v>0</v>
-      </c>
-      <c r="D91" s="10">
+      <c r="D87" s="10">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B72:D72"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B75:D75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6777,22 +6745,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="37"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="50"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="56"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -6899,22 +6867,22 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="49"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="50"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="56"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
@@ -7043,45 +7011,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="37" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7089,8 +7057,8 @@
       <c r="B8" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
@@ -7335,8 +7303,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7347,45 +7315,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="37" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7393,8 +7361,8 @@
       <c r="B8" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
@@ -7577,54 +7545,54 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="36"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="51" t="s">
+      <c r="D36" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="55" t="s">
+      <c r="D37" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="37" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7632,9 +7600,9 @@
       <c r="B38" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="6"/>

</xml_diff>